<commit_message>
Added retry, dataprovider, js actions
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\IdeaProjects\fall_2022_selenium\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299A9A1B-3210-4850-B210-8C88A06E655F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E95269-42BA-4041-AB31-56283D8B7674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{5D387A7A-66E4-47AC-93CF-8AC7DCAA63E7}"/>
+    <workbookView xWindow="-28800" yWindow="345" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{5D387A7A-66E4-47AC-93CF-8AC7DCAA63E7}"/>
   </bookViews>
   <sheets>
     <sheet name="TestRegisterNewAccount" sheetId="1" r:id="rId1"/>
     <sheet name="TestProducts" sheetId="2" r:id="rId2"/>
+    <sheet name="TestProductsDP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Value</t>
   </si>
@@ -48,13 +49,43 @@
     <t>Sheikh</t>
   </si>
   <si>
+    <t>shirt</t>
+  </si>
+  <si>
+    <t>Faded Short Sleeve T-shirts</t>
+  </si>
+  <si>
+    <t>searchTerm</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>dress</t>
   </si>
   <si>
-    <t>Printed Chiffon Dress</t>
+    <t>blouse</t>
+  </si>
+  <si>
+    <t>Blouse</t>
+  </si>
+  <si>
+    <t>Printed Dress</t>
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -757,33 +788,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B41DAE-286C-481D-90AA-D3066797E579}">
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A0C994-5C31-4A10-829E-B6EE3678B743}">
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>